<commit_message>
Added a simple code to read photodiode signals (photoDiodeSimple.m) and Dante's PTB vis_display.m code
</commit_message>
<xml_diff>
--- a/unlock/analysis/andres/Metafiles/unlock-testing-session.xlsx
+++ b/unlock/analysis/andres/Metafiles/unlock-testing-session.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="22995" windowHeight="9525"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="22995" windowHeight="9465"/>
   </bookViews>
   <sheets>
     <sheet name="Unlock Testing " sheetId="1" r:id="rId1"/>
     <sheet name="Subject ID" sheetId="2" r:id="rId2"/>
     <sheet name="Cap Layout" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="68">
   <si>
     <t>No.</t>
   </si>
@@ -198,9 +198,6 @@
     <t>20140106-004</t>
   </si>
   <si>
-    <t>Placing cap</t>
-  </si>
-  <si>
     <t>James</t>
   </si>
   <si>
@@ -219,10 +216,22 @@
     <t>Grid Target at 90 degrees. North.</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Use purple cap!!!!</t>
+    <t>20140121-004</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Used gray cap</t>
+  </si>
+  <si>
+    <t>Planned to used purple cap</t>
+  </si>
+  <si>
+    <t>Who put cap on?</t>
+  </si>
+  <si>
+    <t>James cancelled due to weather conditions expected to happen in the afternoon</t>
   </si>
 </sst>
 </file>
@@ -734,8 +743,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:X13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="690" topLeftCell="A7" activePane="bottomLeft"/>
+      <selection activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +760,7 @@
     <col min="7" max="7" width="9.42578125" style="4" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="4" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="4" customWidth="1"/>
     <col min="11" max="11" width="8.140625" style="4" customWidth="1"/>
     <col min="12" max="12" width="13" style="4" customWidth="1"/>
     <col min="13" max="14" width="12.140625" style="4" customWidth="1"/>
@@ -804,7 +815,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>1</v>
@@ -875,7 +886,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>23</v>
@@ -947,7 +958,7 @@
         <v>47</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>48</v>
@@ -965,7 +976,7 @@
         <v>6</v>
       </c>
       <c r="K6" s="9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L6" s="9" t="s">
         <v>11</v>
@@ -1012,7 +1023,7 @@
         <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>48</v>
@@ -1024,19 +1035,19 @@
         <v>49</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K7" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>21</v>
@@ -1056,7 +1067,7 @@
         <v>64</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U7" s="3"/>
       <c r="V7" s="3" t="s">
@@ -1069,34 +1080,72 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:24" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="11">
         <v>4</v>
       </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
+      <c r="C8" s="9">
+        <v>20140121</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="9">
+        <v>8</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="M8" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="N8" s="9"/>
+      <c r="N8" s="9" t="s">
+        <v>21</v>
+      </c>
       <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="9"/>
+      <c r="P8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="S8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="U8" s="9"/>
-      <c r="V8" s="9"/>
-      <c r="W8" s="9"/>
-      <c r="X8" s="9"/>
+      <c r="V8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="W8" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="X8" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B9" s="10">

</xml_diff>